<commit_message>
más registros de incidencias
</commit_message>
<xml_diff>
--- a/Datos/incidencia.xlsx
+++ b/Datos/incidencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB2B6E6-E10E-47D3-930A-99C7AC922EEC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53E134A-77B1-4EF5-BD27-E335BA1BB433}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="12">
   <si>
     <t>idincidencia</t>
   </si>
@@ -54,12 +54,15 @@
   <si>
     <t>FT</t>
   </si>
+  <si>
+    <t>FD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +200,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -557,7 +566,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -567,6 +576,15 @@
     </xf>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -923,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2911,24 +2929,24 @@
       </c>
     </row>
     <row r="95" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="2">
+      <c r="A95" s="4">
         <v>94</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B95" s="5">
         <v>43229</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D95" s="1"/>
-      <c r="E95" s="2">
-        <v>1</v>
-      </c>
-      <c r="F95" s="2">
-        <v>9</v>
-      </c>
-      <c r="G95" s="2">
-        <v>3</v>
+      <c r="E95" s="4">
+        <v>1</v>
+      </c>
+      <c r="F95" s="4">
+        <v>9</v>
+      </c>
+      <c r="G95" s="4">
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2936,20 +2954,20 @@
         <v>95</v>
       </c>
       <c r="B96" s="3">
-        <v>43230</v>
+        <v>43229</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F96" s="2">
         <v>9</v>
       </c>
       <c r="G96" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2957,14 +2975,14 @@
         <v>96</v>
       </c>
       <c r="B97" s="3">
-        <v>43234</v>
+        <v>43229</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F97" s="2">
         <v>9</v>
@@ -2978,14 +2996,14 @@
         <v>97</v>
       </c>
       <c r="B98" s="3">
-        <v>43236</v>
+        <v>43229</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F98" s="2">
         <v>9</v>
@@ -2999,23 +3017,3174 @@
         <v>98</v>
       </c>
       <c r="B99" s="3">
-        <v>43237</v>
+        <v>43229</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F99" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G99" s="2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="2">
+        <v>99</v>
+      </c>
+      <c r="B100" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" s="1"/>
+      <c r="E100" s="2">
+        <v>6</v>
+      </c>
+      <c r="F100" s="2">
+        <v>9</v>
+      </c>
+      <c r="G100" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="2">
+        <v>100</v>
+      </c>
+      <c r="B101" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" s="1"/>
+      <c r="E101" s="2">
+        <v>7</v>
+      </c>
+      <c r="F101" s="2">
+        <v>9</v>
+      </c>
+      <c r="G101" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="2">
+        <v>101</v>
+      </c>
+      <c r="B102" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" s="1"/>
+      <c r="E102" s="2">
+        <v>8</v>
+      </c>
+      <c r="F102" s="2">
+        <v>9</v>
+      </c>
+      <c r="G102" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="2">
+        <v>102</v>
+      </c>
+      <c r="B103" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" s="1"/>
+      <c r="E103" s="2">
+        <v>9</v>
+      </c>
+      <c r="F103" s="2">
+        <v>9</v>
+      </c>
+      <c r="G103" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="2">
+        <v>103</v>
+      </c>
+      <c r="B104" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104" s="1"/>
+      <c r="E104" s="2">
+        <v>10</v>
+      </c>
+      <c r="F104" s="2">
+        <v>9</v>
+      </c>
+      <c r="G104" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="2">
+        <v>104</v>
+      </c>
+      <c r="B105" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" s="1"/>
+      <c r="E105" s="2">
+        <v>11</v>
+      </c>
+      <c r="F105" s="2">
+        <v>9</v>
+      </c>
+      <c r="G105" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="2">
+        <v>105</v>
+      </c>
+      <c r="B106" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106" s="1"/>
+      <c r="E106" s="2">
+        <v>12</v>
+      </c>
+      <c r="F106" s="2">
+        <v>9</v>
+      </c>
+      <c r="G106" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="2">
+        <v>106</v>
+      </c>
+      <c r="B107" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107" s="1"/>
+      <c r="E107" s="2">
+        <v>13</v>
+      </c>
+      <c r="F107" s="2">
+        <v>9</v>
+      </c>
+      <c r="G107" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="2">
+        <v>107</v>
+      </c>
+      <c r="B108" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108" s="1"/>
+      <c r="E108" s="2">
+        <v>14</v>
+      </c>
+      <c r="F108" s="2">
+        <v>9</v>
+      </c>
+      <c r="G108" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="2">
+        <v>108</v>
+      </c>
+      <c r="B109" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" s="1"/>
+      <c r="E109" s="2">
+        <v>15</v>
+      </c>
+      <c r="F109" s="2">
+        <v>9</v>
+      </c>
+      <c r="G109" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="2">
+        <v>109</v>
+      </c>
+      <c r="B110" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" s="1"/>
+      <c r="E110" s="2">
+        <v>243</v>
+      </c>
+      <c r="F110" s="2">
+        <v>9</v>
+      </c>
+      <c r="G110" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="2">
+        <v>110</v>
+      </c>
+      <c r="B111" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" s="1"/>
+      <c r="E111" s="2">
+        <v>244</v>
+      </c>
+      <c r="F111" s="2">
+        <v>9</v>
+      </c>
+      <c r="G111" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="2">
+        <v>111</v>
+      </c>
+      <c r="B112" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" s="1"/>
+      <c r="E112" s="2">
+        <v>245</v>
+      </c>
+      <c r="F112" s="2">
+        <v>9</v>
+      </c>
+      <c r="G112" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="2">
+        <v>112</v>
+      </c>
+      <c r="B113" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113" s="1"/>
+      <c r="E113" s="2">
+        <v>246</v>
+      </c>
+      <c r="F113" s="2">
+        <v>9</v>
+      </c>
+      <c r="G113" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="2">
+        <v>113</v>
+      </c>
+      <c r="B114" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114" s="1"/>
+      <c r="E114" s="2">
+        <v>247</v>
+      </c>
+      <c r="F114" s="2">
+        <v>9</v>
+      </c>
+      <c r="G114" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="2">
+        <v>114</v>
+      </c>
+      <c r="B115" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D115" s="1"/>
+      <c r="E115" s="2">
+        <v>248</v>
+      </c>
+      <c r="F115" s="2">
+        <v>9</v>
+      </c>
+      <c r="G115" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="2">
+        <v>115</v>
+      </c>
+      <c r="B116" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D116" s="1"/>
+      <c r="E116" s="2">
+        <v>249</v>
+      </c>
+      <c r="F116" s="2">
+        <v>9</v>
+      </c>
+      <c r="G116" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="2">
+        <v>116</v>
+      </c>
+      <c r="B117" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D117" s="1"/>
+      <c r="E117" s="2">
+        <v>250</v>
+      </c>
+      <c r="F117" s="2">
+        <v>9</v>
+      </c>
+      <c r="G117" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="2">
+        <v>117</v>
+      </c>
+      <c r="B118" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" s="1"/>
+      <c r="E118" s="2">
+        <v>251</v>
+      </c>
+      <c r="F118" s="2">
+        <v>9</v>
+      </c>
+      <c r="G118" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="2">
+        <v>118</v>
+      </c>
+      <c r="B119" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D119" s="1"/>
+      <c r="E119" s="2">
+        <v>252</v>
+      </c>
+      <c r="F119" s="2">
+        <v>9</v>
+      </c>
+      <c r="G119" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="2">
+        <v>119</v>
+      </c>
+      <c r="B120" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D120" s="1"/>
+      <c r="E120" s="2">
+        <v>253</v>
+      </c>
+      <c r="F120" s="2">
+        <v>9</v>
+      </c>
+      <c r="G120" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="2">
+        <v>120</v>
+      </c>
+      <c r="B121" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D121" s="1"/>
+      <c r="E121" s="2">
+        <v>254</v>
+      </c>
+      <c r="F121" s="2">
+        <v>9</v>
+      </c>
+      <c r="G121" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="2">
+        <v>121</v>
+      </c>
+      <c r="B122" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D122" s="1"/>
+      <c r="E122" s="2">
+        <v>255</v>
+      </c>
+      <c r="F122" s="2">
+        <v>9</v>
+      </c>
+      <c r="G122" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="2">
+        <v>122</v>
+      </c>
+      <c r="B123" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D123" s="1"/>
+      <c r="E123" s="2">
+        <v>256</v>
+      </c>
+      <c r="F123" s="2">
+        <v>9</v>
+      </c>
+      <c r="G123" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="2">
+        <v>123</v>
+      </c>
+      <c r="B124" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D124" s="1"/>
+      <c r="E124" s="2">
+        <v>257</v>
+      </c>
+      <c r="F124" s="2">
+        <v>9</v>
+      </c>
+      <c r="G124" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="2">
+        <v>124</v>
+      </c>
+      <c r="B125" s="3">
+        <v>43229</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D125" s="1"/>
+      <c r="E125" s="2">
+        <v>258</v>
+      </c>
+      <c r="F125" s="2">
+        <v>9</v>
+      </c>
+      <c r="G125" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="2">
+        <v>125</v>
+      </c>
+      <c r="B126" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D126" s="1"/>
+      <c r="E126" s="2">
+        <v>1</v>
+      </c>
+      <c r="F126" s="2">
+        <v>9</v>
+      </c>
+      <c r="G126" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="2">
+        <v>126</v>
+      </c>
+      <c r="B127" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D127" s="1"/>
+      <c r="E127" s="2">
+        <v>2</v>
+      </c>
+      <c r="F127" s="2">
+        <v>9</v>
+      </c>
+      <c r="G127" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="2">
+        <v>127</v>
+      </c>
+      <c r="B128" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D128" s="1"/>
+      <c r="E128" s="2">
+        <v>3</v>
+      </c>
+      <c r="F128" s="2">
+        <v>9</v>
+      </c>
+      <c r="G128" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="2">
+        <v>128</v>
+      </c>
+      <c r="B129" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D129" s="1"/>
+      <c r="E129" s="2">
+        <v>4</v>
+      </c>
+      <c r="F129" s="2">
+        <v>9</v>
+      </c>
+      <c r="G129" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="2">
+        <v>129</v>
+      </c>
+      <c r="B130" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D130" s="1"/>
+      <c r="E130" s="2">
+        <v>5</v>
+      </c>
+      <c r="F130" s="2">
+        <v>9</v>
+      </c>
+      <c r="G130" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="2">
+        <v>130</v>
+      </c>
+      <c r="B131" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D131" s="1"/>
+      <c r="E131" s="2">
+        <v>6</v>
+      </c>
+      <c r="F131" s="2">
+        <v>9</v>
+      </c>
+      <c r="G131" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="2">
+        <v>131</v>
+      </c>
+      <c r="B132" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D132" s="1"/>
+      <c r="E132" s="2">
+        <v>7</v>
+      </c>
+      <c r="F132" s="2">
+        <v>9</v>
+      </c>
+      <c r="G132" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="2">
+        <v>132</v>
+      </c>
+      <c r="B133" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D133" s="1"/>
+      <c r="E133" s="2">
+        <v>8</v>
+      </c>
+      <c r="F133" s="2">
+        <v>9</v>
+      </c>
+      <c r="G133" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="2">
+        <v>133</v>
+      </c>
+      <c r="B134" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D134" s="1"/>
+      <c r="E134" s="2">
+        <v>9</v>
+      </c>
+      <c r="F134" s="2">
+        <v>9</v>
+      </c>
+      <c r="G134" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="2">
+        <v>134</v>
+      </c>
+      <c r="B135" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D135" s="1"/>
+      <c r="E135" s="2">
+        <v>10</v>
+      </c>
+      <c r="F135" s="2">
+        <v>9</v>
+      </c>
+      <c r="G135" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="2">
+        <v>135</v>
+      </c>
+      <c r="B136" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136" s="1"/>
+      <c r="E136" s="2">
+        <v>11</v>
+      </c>
+      <c r="F136" s="2">
+        <v>9</v>
+      </c>
+      <c r="G136" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="2">
+        <v>136</v>
+      </c>
+      <c r="B137" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137" s="1"/>
+      <c r="E137" s="2">
+        <v>12</v>
+      </c>
+      <c r="F137" s="2">
+        <v>9</v>
+      </c>
+      <c r="G137" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="2">
+        <v>137</v>
+      </c>
+      <c r="B138" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D138" s="1"/>
+      <c r="E138" s="2">
+        <v>13</v>
+      </c>
+      <c r="F138" s="2">
+        <v>9</v>
+      </c>
+      <c r="G138" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="2">
+        <v>138</v>
+      </c>
+      <c r="B139" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D139" s="1"/>
+      <c r="E139" s="2">
+        <v>14</v>
+      </c>
+      <c r="F139" s="2">
+        <v>9</v>
+      </c>
+      <c r="G139" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="2">
+        <v>139</v>
+      </c>
+      <c r="B140" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D140" s="1"/>
+      <c r="E140" s="2">
+        <v>15</v>
+      </c>
+      <c r="F140" s="2">
+        <v>9</v>
+      </c>
+      <c r="G140" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="2">
+        <v>140</v>
+      </c>
+      <c r="B141" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D141" s="1"/>
+      <c r="E141" s="2">
+        <v>243</v>
+      </c>
+      <c r="F141" s="2">
+        <v>9</v>
+      </c>
+      <c r="G141" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="2">
+        <v>141</v>
+      </c>
+      <c r="B142" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D142" s="1"/>
+      <c r="E142" s="2">
+        <v>244</v>
+      </c>
+      <c r="F142" s="2">
+        <v>9</v>
+      </c>
+      <c r="G142" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="2">
+        <v>142</v>
+      </c>
+      <c r="B143" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D143" s="1"/>
+      <c r="E143" s="2">
+        <v>245</v>
+      </c>
+      <c r="F143" s="2">
+        <v>9</v>
+      </c>
+      <c r="G143" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="2">
+        <v>143</v>
+      </c>
+      <c r="B144" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D144" s="1"/>
+      <c r="E144" s="2">
+        <v>246</v>
+      </c>
+      <c r="F144" s="2">
+        <v>9</v>
+      </c>
+      <c r="G144" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="2">
+        <v>144</v>
+      </c>
+      <c r="B145" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D145" s="1"/>
+      <c r="E145" s="2">
+        <v>247</v>
+      </c>
+      <c r="F145" s="2">
+        <v>9</v>
+      </c>
+      <c r="G145" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="2">
+        <v>145</v>
+      </c>
+      <c r="B146" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D146" s="1"/>
+      <c r="E146" s="2">
+        <v>248</v>
+      </c>
+      <c r="F146" s="2">
+        <v>9</v>
+      </c>
+      <c r="G146" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="2">
+        <v>146</v>
+      </c>
+      <c r="B147" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D147" s="1"/>
+      <c r="E147" s="2">
+        <v>249</v>
+      </c>
+      <c r="F147" s="2">
+        <v>9</v>
+      </c>
+      <c r="G147" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="2">
+        <v>147</v>
+      </c>
+      <c r="B148" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D148" s="1"/>
+      <c r="E148" s="2">
+        <v>250</v>
+      </c>
+      <c r="F148" s="2">
+        <v>9</v>
+      </c>
+      <c r="G148" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="2">
+        <v>148</v>
+      </c>
+      <c r="B149" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D149" s="1"/>
+      <c r="E149" s="2">
+        <v>251</v>
+      </c>
+      <c r="F149" s="2">
+        <v>9</v>
+      </c>
+      <c r="G149" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="2">
+        <v>149</v>
+      </c>
+      <c r="B150" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D150" s="1"/>
+      <c r="E150" s="2">
+        <v>252</v>
+      </c>
+      <c r="F150" s="2">
+        <v>9</v>
+      </c>
+      <c r="G150" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="2">
+        <v>150</v>
+      </c>
+      <c r="B151" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D151" s="1"/>
+      <c r="E151" s="2">
+        <v>253</v>
+      </c>
+      <c r="F151" s="2">
+        <v>9</v>
+      </c>
+      <c r="G151" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="2">
+        <v>151</v>
+      </c>
+      <c r="B152" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D152" s="1"/>
+      <c r="E152" s="2">
+        <v>254</v>
+      </c>
+      <c r="F152" s="2">
+        <v>9</v>
+      </c>
+      <c r="G152" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="2">
+        <v>152</v>
+      </c>
+      <c r="B153" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D153" s="1"/>
+      <c r="E153" s="2">
+        <v>255</v>
+      </c>
+      <c r="F153" s="2">
+        <v>9</v>
+      </c>
+      <c r="G153" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="2">
+        <v>153</v>
+      </c>
+      <c r="B154" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D154" s="1"/>
+      <c r="E154" s="2">
+        <v>256</v>
+      </c>
+      <c r="F154" s="2">
+        <v>9</v>
+      </c>
+      <c r="G154" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="2">
+        <v>154</v>
+      </c>
+      <c r="B155" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D155" s="1"/>
+      <c r="E155" s="2">
+        <v>257</v>
+      </c>
+      <c r="F155" s="2">
+        <v>9</v>
+      </c>
+      <c r="G155" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="2">
+        <v>155</v>
+      </c>
+      <c r="B156" s="3">
+        <v>43230</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D156" s="1"/>
+      <c r="E156" s="2">
+        <v>258</v>
+      </c>
+      <c r="F156" s="2">
+        <v>9</v>
+      </c>
+      <c r="G156" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="2">
+        <v>156</v>
+      </c>
+      <c r="B157" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C157" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D157" s="1"/>
+      <c r="E157" s="2">
+        <v>1</v>
+      </c>
+      <c r="F157" s="2">
+        <v>9</v>
+      </c>
+      <c r="G157" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="2">
+        <v>157</v>
+      </c>
+      <c r="B158" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D158" s="1"/>
+      <c r="E158" s="2">
+        <v>2</v>
+      </c>
+      <c r="F158" s="2">
+        <v>9</v>
+      </c>
+      <c r="G158" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="2">
+        <v>158</v>
+      </c>
+      <c r="B159" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D159" s="1"/>
+      <c r="E159" s="2">
+        <v>3</v>
+      </c>
+      <c r="F159" s="2">
+        <v>9</v>
+      </c>
+      <c r="G159" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="2">
+        <v>159</v>
+      </c>
+      <c r="B160" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D160" s="1"/>
+      <c r="E160" s="2">
+        <v>4</v>
+      </c>
+      <c r="F160" s="2">
+        <v>9</v>
+      </c>
+      <c r="G160" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="2">
+        <v>160</v>
+      </c>
+      <c r="B161" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D161" s="1"/>
+      <c r="E161" s="2">
+        <v>5</v>
+      </c>
+      <c r="F161" s="2">
+        <v>9</v>
+      </c>
+      <c r="G161" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="2">
+        <v>161</v>
+      </c>
+      <c r="B162" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D162" s="1"/>
+      <c r="E162" s="2">
+        <v>6</v>
+      </c>
+      <c r="F162" s="2">
+        <v>9</v>
+      </c>
+      <c r="G162" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="2">
+        <v>162</v>
+      </c>
+      <c r="B163" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D163" s="1"/>
+      <c r="E163" s="2">
+        <v>7</v>
+      </c>
+      <c r="F163" s="2">
+        <v>9</v>
+      </c>
+      <c r="G163" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="2">
+        <v>163</v>
+      </c>
+      <c r="B164" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D164" s="1"/>
+      <c r="E164" s="2">
+        <v>8</v>
+      </c>
+      <c r="F164" s="2">
+        <v>9</v>
+      </c>
+      <c r="G164" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="2">
+        <v>164</v>
+      </c>
+      <c r="B165" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D165" s="1"/>
+      <c r="E165" s="2">
+        <v>9</v>
+      </c>
+      <c r="F165" s="2">
+        <v>9</v>
+      </c>
+      <c r="G165" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="2">
+        <v>165</v>
+      </c>
+      <c r="B166" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D166" s="1"/>
+      <c r="E166" s="2">
+        <v>10</v>
+      </c>
+      <c r="F166" s="2">
+        <v>9</v>
+      </c>
+      <c r="G166" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="2">
+        <v>166</v>
+      </c>
+      <c r="B167" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D167" s="1"/>
+      <c r="E167" s="2">
+        <v>11</v>
+      </c>
+      <c r="F167" s="2">
+        <v>9</v>
+      </c>
+      <c r="G167" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="2">
+        <v>167</v>
+      </c>
+      <c r="B168" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168" s="1"/>
+      <c r="E168" s="2">
+        <v>12</v>
+      </c>
+      <c r="F168" s="2">
+        <v>9</v>
+      </c>
+      <c r="G168" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="2">
+        <v>168</v>
+      </c>
+      <c r="B169" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D169" s="1"/>
+      <c r="E169" s="2">
+        <v>13</v>
+      </c>
+      <c r="F169" s="2">
+        <v>9</v>
+      </c>
+      <c r="G169" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="2">
+        <v>169</v>
+      </c>
+      <c r="B170" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D170" s="1"/>
+      <c r="E170" s="2">
+        <v>14</v>
+      </c>
+      <c r="F170" s="2">
+        <v>9</v>
+      </c>
+      <c r="G170" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="2">
+        <v>170</v>
+      </c>
+      <c r="B171" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D171" s="1"/>
+      <c r="E171" s="2">
+        <v>15</v>
+      </c>
+      <c r="F171" s="2">
+        <v>9</v>
+      </c>
+      <c r="G171" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="2">
+        <v>171</v>
+      </c>
+      <c r="B172" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172" s="1"/>
+      <c r="E172" s="2">
+        <v>243</v>
+      </c>
+      <c r="F172" s="2">
+        <v>9</v>
+      </c>
+      <c r="G172" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="2">
+        <v>172</v>
+      </c>
+      <c r="B173" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D173" s="1"/>
+      <c r="E173" s="2">
+        <v>244</v>
+      </c>
+      <c r="F173" s="2">
+        <v>9</v>
+      </c>
+      <c r="G173" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="2">
+        <v>173</v>
+      </c>
+      <c r="B174" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D174" s="1"/>
+      <c r="E174" s="2">
+        <v>245</v>
+      </c>
+      <c r="F174" s="2">
+        <v>9</v>
+      </c>
+      <c r="G174" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="2">
+        <v>174</v>
+      </c>
+      <c r="B175" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D175" s="1"/>
+      <c r="E175" s="2">
+        <v>246</v>
+      </c>
+      <c r="F175" s="2">
+        <v>9</v>
+      </c>
+      <c r="G175" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="2">
+        <v>175</v>
+      </c>
+      <c r="B176" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D176" s="1"/>
+      <c r="E176" s="2">
+        <v>247</v>
+      </c>
+      <c r="F176" s="2">
+        <v>9</v>
+      </c>
+      <c r="G176" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="2">
+        <v>176</v>
+      </c>
+      <c r="B177" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D177" s="1"/>
+      <c r="E177" s="2">
+        <v>248</v>
+      </c>
+      <c r="F177" s="2">
+        <v>9</v>
+      </c>
+      <c r="G177" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="2">
+        <v>177</v>
+      </c>
+      <c r="B178" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D178" s="1"/>
+      <c r="E178" s="2">
+        <v>249</v>
+      </c>
+      <c r="F178" s="2">
+        <v>9</v>
+      </c>
+      <c r="G178" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="2">
+        <v>178</v>
+      </c>
+      <c r="B179" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D179" s="1"/>
+      <c r="E179" s="2">
+        <v>250</v>
+      </c>
+      <c r="F179" s="2">
+        <v>9</v>
+      </c>
+      <c r="G179" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="2">
+        <v>179</v>
+      </c>
+      <c r="B180" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D180" s="1"/>
+      <c r="E180" s="2">
+        <v>251</v>
+      </c>
+      <c r="F180" s="2">
+        <v>9</v>
+      </c>
+      <c r="G180" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="2">
+        <v>180</v>
+      </c>
+      <c r="B181" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D181" s="1"/>
+      <c r="E181" s="2">
+        <v>252</v>
+      </c>
+      <c r="F181" s="2">
+        <v>9</v>
+      </c>
+      <c r="G181" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="2">
+        <v>181</v>
+      </c>
+      <c r="B182" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D182" s="1"/>
+      <c r="E182" s="2">
+        <v>253</v>
+      </c>
+      <c r="F182" s="2">
+        <v>9</v>
+      </c>
+      <c r="G182" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="2">
+        <v>182</v>
+      </c>
+      <c r="B183" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D183" s="1"/>
+      <c r="E183" s="2">
+        <v>254</v>
+      </c>
+      <c r="F183" s="2">
+        <v>9</v>
+      </c>
+      <c r="G183" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="2">
+        <v>183</v>
+      </c>
+      <c r="B184" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D184" s="1"/>
+      <c r="E184" s="2">
+        <v>255</v>
+      </c>
+      <c r="F184" s="2">
+        <v>9</v>
+      </c>
+      <c r="G184" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="2">
+        <v>184</v>
+      </c>
+      <c r="B185" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D185" s="1"/>
+      <c r="E185" s="2">
+        <v>256</v>
+      </c>
+      <c r="F185" s="2">
+        <v>9</v>
+      </c>
+      <c r="G185" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="2">
+        <v>185</v>
+      </c>
+      <c r="B186" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D186" s="1"/>
+      <c r="E186" s="2">
+        <v>257</v>
+      </c>
+      <c r="F186" s="2">
+        <v>9</v>
+      </c>
+      <c r="G186" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="2">
+        <v>186</v>
+      </c>
+      <c r="B187" s="3">
+        <v>43234</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D187" s="1"/>
+      <c r="E187" s="2">
+        <v>258</v>
+      </c>
+      <c r="F187" s="2">
+        <v>9</v>
+      </c>
+      <c r="G187" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="2">
+        <v>187</v>
+      </c>
+      <c r="B188" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C188" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D188" s="1"/>
+      <c r="E188" s="2">
+        <v>1</v>
+      </c>
+      <c r="F188" s="2">
+        <v>10</v>
+      </c>
+      <c r="G188" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="2">
+        <v>188</v>
+      </c>
+      <c r="B189" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D189" s="1"/>
+      <c r="E189" s="2">
+        <v>2</v>
+      </c>
+      <c r="F189" s="2">
+        <v>10</v>
+      </c>
+      <c r="G189" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="2">
+        <v>189</v>
+      </c>
+      <c r="B190" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D190" s="1"/>
+      <c r="E190" s="2">
+        <v>3</v>
+      </c>
+      <c r="F190" s="2">
+        <v>10</v>
+      </c>
+      <c r="G190" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="2">
+        <v>190</v>
+      </c>
+      <c r="B191" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D191" s="1"/>
+      <c r="E191" s="2">
+        <v>4</v>
+      </c>
+      <c r="F191" s="2">
+        <v>10</v>
+      </c>
+      <c r="G191" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="2">
+        <v>191</v>
+      </c>
+      <c r="B192" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D192" s="1"/>
+      <c r="E192" s="2">
+        <v>5</v>
+      </c>
+      <c r="F192" s="2">
+        <v>10</v>
+      </c>
+      <c r="G192" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="2">
+        <v>192</v>
+      </c>
+      <c r="B193" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D193" s="1"/>
+      <c r="E193" s="2">
+        <v>6</v>
+      </c>
+      <c r="F193" s="2">
+        <v>10</v>
+      </c>
+      <c r="G193" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="2">
+        <v>193</v>
+      </c>
+      <c r="B194" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D194" s="1"/>
+      <c r="E194" s="2">
+        <v>7</v>
+      </c>
+      <c r="F194" s="2">
+        <v>10</v>
+      </c>
+      <c r="G194" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="2">
+        <v>194</v>
+      </c>
+      <c r="B195" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D195" s="1"/>
+      <c r="E195" s="2">
+        <v>8</v>
+      </c>
+      <c r="F195" s="2">
+        <v>10</v>
+      </c>
+      <c r="G195" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="2">
+        <v>195</v>
+      </c>
+      <c r="B196" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D196" s="1"/>
+      <c r="E196" s="2">
+        <v>9</v>
+      </c>
+      <c r="F196" s="2">
+        <v>10</v>
+      </c>
+      <c r="G196" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="2">
+        <v>196</v>
+      </c>
+      <c r="B197" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D197" s="1"/>
+      <c r="E197" s="2">
+        <v>10</v>
+      </c>
+      <c r="F197" s="2">
+        <v>10</v>
+      </c>
+      <c r="G197" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="2">
+        <v>197</v>
+      </c>
+      <c r="B198" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D198" s="1"/>
+      <c r="E198" s="2">
+        <v>11</v>
+      </c>
+      <c r="F198" s="2">
+        <v>10</v>
+      </c>
+      <c r="G198" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="2">
+        <v>198</v>
+      </c>
+      <c r="B199" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D199" s="1"/>
+      <c r="E199" s="2">
+        <v>12</v>
+      </c>
+      <c r="F199" s="2">
+        <v>10</v>
+      </c>
+      <c r="G199" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="2">
+        <v>199</v>
+      </c>
+      <c r="B200" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D200" s="1"/>
+      <c r="E200" s="2">
+        <v>13</v>
+      </c>
+      <c r="F200" s="2">
+        <v>10</v>
+      </c>
+      <c r="G200" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="2">
+        <v>200</v>
+      </c>
+      <c r="B201" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D201" s="1"/>
+      <c r="E201" s="2">
+        <v>14</v>
+      </c>
+      <c r="F201" s="2">
+        <v>10</v>
+      </c>
+      <c r="G201" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="2">
+        <v>201</v>
+      </c>
+      <c r="B202" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D202" s="1"/>
+      <c r="E202" s="2">
+        <v>15</v>
+      </c>
+      <c r="F202" s="2">
+        <v>10</v>
+      </c>
+      <c r="G202" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A203" s="2">
+        <v>202</v>
+      </c>
+      <c r="B203" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D203" s="1"/>
+      <c r="E203" s="2">
+        <v>243</v>
+      </c>
+      <c r="F203" s="2">
+        <v>10</v>
+      </c>
+      <c r="G203" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="2">
+        <v>203</v>
+      </c>
+      <c r="B204" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D204" s="1"/>
+      <c r="E204" s="2">
+        <v>244</v>
+      </c>
+      <c r="F204" s="2">
+        <v>10</v>
+      </c>
+      <c r="G204" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="2">
+        <v>204</v>
+      </c>
+      <c r="B205" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D205" s="1"/>
+      <c r="E205" s="2">
+        <v>245</v>
+      </c>
+      <c r="F205" s="2">
+        <v>10</v>
+      </c>
+      <c r="G205" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="2">
+        <v>205</v>
+      </c>
+      <c r="B206" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D206" s="1"/>
+      <c r="E206" s="2">
+        <v>246</v>
+      </c>
+      <c r="F206" s="2">
+        <v>10</v>
+      </c>
+      <c r="G206" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="2">
+        <v>206</v>
+      </c>
+      <c r="B207" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D207" s="1"/>
+      <c r="E207" s="2">
+        <v>247</v>
+      </c>
+      <c r="F207" s="2">
+        <v>10</v>
+      </c>
+      <c r="G207" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="2">
+        <v>207</v>
+      </c>
+      <c r="B208" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D208" s="1"/>
+      <c r="E208" s="2">
+        <v>248</v>
+      </c>
+      <c r="F208" s="2">
+        <v>10</v>
+      </c>
+      <c r="G208" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A209" s="2">
+        <v>208</v>
+      </c>
+      <c r="B209" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D209" s="1"/>
+      <c r="E209" s="2">
+        <v>249</v>
+      </c>
+      <c r="F209" s="2">
+        <v>10</v>
+      </c>
+      <c r="G209" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="2">
+        <v>209</v>
+      </c>
+      <c r="B210" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D210" s="1"/>
+      <c r="E210" s="2">
+        <v>250</v>
+      </c>
+      <c r="F210" s="2">
+        <v>10</v>
+      </c>
+      <c r="G210" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A211" s="2">
+        <v>210</v>
+      </c>
+      <c r="B211" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D211" s="1"/>
+      <c r="E211" s="2">
+        <v>251</v>
+      </c>
+      <c r="F211" s="2">
+        <v>10</v>
+      </c>
+      <c r="G211" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A212" s="2">
+        <v>211</v>
+      </c>
+      <c r="B212" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D212" s="1"/>
+      <c r="E212" s="2">
+        <v>252</v>
+      </c>
+      <c r="F212" s="2">
+        <v>10</v>
+      </c>
+      <c r="G212" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A213" s="2">
+        <v>212</v>
+      </c>
+      <c r="B213" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D213" s="1"/>
+      <c r="E213" s="2">
+        <v>253</v>
+      </c>
+      <c r="F213" s="2">
+        <v>10</v>
+      </c>
+      <c r="G213" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="2">
+        <v>213</v>
+      </c>
+      <c r="B214" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D214" s="1"/>
+      <c r="E214" s="2">
+        <v>254</v>
+      </c>
+      <c r="F214" s="2">
+        <v>10</v>
+      </c>
+      <c r="G214" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A215" s="2">
+        <v>214</v>
+      </c>
+      <c r="B215" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D215" s="1"/>
+      <c r="E215" s="2">
+        <v>255</v>
+      </c>
+      <c r="F215" s="2">
+        <v>10</v>
+      </c>
+      <c r="G215" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A216" s="2">
+        <v>215</v>
+      </c>
+      <c r="B216" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D216" s="1"/>
+      <c r="E216" s="2">
+        <v>256</v>
+      </c>
+      <c r="F216" s="2">
+        <v>10</v>
+      </c>
+      <c r="G216" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="2">
+        <v>216</v>
+      </c>
+      <c r="B217" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D217" s="1"/>
+      <c r="E217" s="2">
+        <v>257</v>
+      </c>
+      <c r="F217" s="2">
+        <v>10</v>
+      </c>
+      <c r="G217" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="2">
+        <v>217</v>
+      </c>
+      <c r="B218" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D218" s="1"/>
+      <c r="E218" s="2">
+        <v>258</v>
+      </c>
+      <c r="F218" s="2">
+        <v>10</v>
+      </c>
+      <c r="G218" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="2">
+        <v>218</v>
+      </c>
+      <c r="B219" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C219" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D219" s="1"/>
+      <c r="E219" s="2">
+        <v>1</v>
+      </c>
+      <c r="F219" s="2">
+        <v>10</v>
+      </c>
+      <c r="G219" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A220" s="2">
+        <v>219</v>
+      </c>
+      <c r="B220" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D220" s="1"/>
+      <c r="E220" s="2">
+        <v>2</v>
+      </c>
+      <c r="F220" s="2">
+        <v>10</v>
+      </c>
+      <c r="G220" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="2">
+        <v>220</v>
+      </c>
+      <c r="B221" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D221" s="1"/>
+      <c r="E221" s="2">
+        <v>3</v>
+      </c>
+      <c r="F221" s="2">
+        <v>10</v>
+      </c>
+      <c r="G221" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="2">
+        <v>221</v>
+      </c>
+      <c r="B222" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D222" s="1"/>
+      <c r="E222" s="2">
+        <v>4</v>
+      </c>
+      <c r="F222" s="2">
+        <v>10</v>
+      </c>
+      <c r="G222" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="2">
+        <v>222</v>
+      </c>
+      <c r="B223" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D223" s="1"/>
+      <c r="E223" s="2">
+        <v>5</v>
+      </c>
+      <c r="F223" s="2">
+        <v>10</v>
+      </c>
+      <c r="G223" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A224" s="2">
+        <v>223</v>
+      </c>
+      <c r="B224" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D224" s="1"/>
+      <c r="E224" s="2">
+        <v>6</v>
+      </c>
+      <c r="F224" s="2">
+        <v>10</v>
+      </c>
+      <c r="G224" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="2">
+        <v>224</v>
+      </c>
+      <c r="B225" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D225" s="1"/>
+      <c r="E225" s="2">
+        <v>7</v>
+      </c>
+      <c r="F225" s="2">
+        <v>10</v>
+      </c>
+      <c r="G225" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="2">
+        <v>225</v>
+      </c>
+      <c r="B226" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D226" s="1"/>
+      <c r="E226" s="2">
+        <v>8</v>
+      </c>
+      <c r="F226" s="2">
+        <v>10</v>
+      </c>
+      <c r="G226" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="2">
+        <v>226</v>
+      </c>
+      <c r="B227" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D227" s="1"/>
+      <c r="E227" s="2">
+        <v>9</v>
+      </c>
+      <c r="F227" s="2">
+        <v>10</v>
+      </c>
+      <c r="G227" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="2">
+        <v>227</v>
+      </c>
+      <c r="B228" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D228" s="1"/>
+      <c r="E228" s="2">
+        <v>10</v>
+      </c>
+      <c r="F228" s="2">
+        <v>10</v>
+      </c>
+      <c r="G228" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="2">
+        <v>228</v>
+      </c>
+      <c r="B229" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D229" s="1"/>
+      <c r="E229" s="2">
+        <v>11</v>
+      </c>
+      <c r="F229" s="2">
+        <v>10</v>
+      </c>
+      <c r="G229" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="2">
+        <v>229</v>
+      </c>
+      <c r="B230" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D230" s="1"/>
+      <c r="E230" s="2">
+        <v>12</v>
+      </c>
+      <c r="F230" s="2">
+        <v>10</v>
+      </c>
+      <c r="G230" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A231" s="2">
+        <v>230</v>
+      </c>
+      <c r="B231" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D231" s="1"/>
+      <c r="E231" s="2">
+        <v>13</v>
+      </c>
+      <c r="F231" s="2">
+        <v>10</v>
+      </c>
+      <c r="G231" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A232" s="2">
+        <v>231</v>
+      </c>
+      <c r="B232" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D232" s="1"/>
+      <c r="E232" s="2">
+        <v>14</v>
+      </c>
+      <c r="F232" s="2">
+        <v>10</v>
+      </c>
+      <c r="G232" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="2">
+        <v>232</v>
+      </c>
+      <c r="B233" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D233" s="1"/>
+      <c r="E233" s="2">
+        <v>15</v>
+      </c>
+      <c r="F233" s="2">
+        <v>10</v>
+      </c>
+      <c r="G233" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="2">
+        <v>233</v>
+      </c>
+      <c r="B234" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D234" s="1"/>
+      <c r="E234" s="2">
+        <v>243</v>
+      </c>
+      <c r="F234" s="2">
+        <v>10</v>
+      </c>
+      <c r="G234" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="2">
+        <v>234</v>
+      </c>
+      <c r="B235" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D235" s="1"/>
+      <c r="E235" s="2">
+        <v>244</v>
+      </c>
+      <c r="F235" s="2">
+        <v>10</v>
+      </c>
+      <c r="G235" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="2">
+        <v>235</v>
+      </c>
+      <c r="B236" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D236" s="1"/>
+      <c r="E236" s="2">
+        <v>245</v>
+      </c>
+      <c r="F236" s="2">
+        <v>10</v>
+      </c>
+      <c r="G236" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="2">
+        <v>236</v>
+      </c>
+      <c r="B237" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D237" s="1"/>
+      <c r="E237" s="2">
+        <v>246</v>
+      </c>
+      <c r="F237" s="2">
+        <v>10</v>
+      </c>
+      <c r="G237" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="2">
+        <v>237</v>
+      </c>
+      <c r="B238" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D238" s="1"/>
+      <c r="E238" s="2">
+        <v>247</v>
+      </c>
+      <c r="F238" s="2">
+        <v>10</v>
+      </c>
+      <c r="G238" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="2">
+        <v>238</v>
+      </c>
+      <c r="B239" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D239" s="1"/>
+      <c r="E239" s="2">
+        <v>248</v>
+      </c>
+      <c r="F239" s="2">
+        <v>10</v>
+      </c>
+      <c r="G239" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="2">
+        <v>239</v>
+      </c>
+      <c r="B240" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D240" s="1"/>
+      <c r="E240" s="2">
+        <v>249</v>
+      </c>
+      <c r="F240" s="2">
+        <v>10</v>
+      </c>
+      <c r="G240" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="2">
+        <v>240</v>
+      </c>
+      <c r="B241" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D241" s="1"/>
+      <c r="E241" s="2">
+        <v>250</v>
+      </c>
+      <c r="F241" s="2">
+        <v>10</v>
+      </c>
+      <c r="G241" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="2">
+        <v>241</v>
+      </c>
+      <c r="B242" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D242" s="1"/>
+      <c r="E242" s="2">
+        <v>251</v>
+      </c>
+      <c r="F242" s="2">
+        <v>10</v>
+      </c>
+      <c r="G242" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A243" s="2">
+        <v>242</v>
+      </c>
+      <c r="B243" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D243" s="1"/>
+      <c r="E243" s="2">
+        <v>252</v>
+      </c>
+      <c r="F243" s="2">
+        <v>10</v>
+      </c>
+      <c r="G243" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A244" s="2">
+        <v>243</v>
+      </c>
+      <c r="B244" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D244" s="1"/>
+      <c r="E244" s="2">
+        <v>253</v>
+      </c>
+      <c r="F244" s="2">
+        <v>10</v>
+      </c>
+      <c r="G244" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="2">
+        <v>244</v>
+      </c>
+      <c r="B245" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D245" s="1"/>
+      <c r="E245" s="2">
+        <v>254</v>
+      </c>
+      <c r="F245" s="2">
+        <v>10</v>
+      </c>
+      <c r="G245" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A246" s="2">
+        <v>245</v>
+      </c>
+      <c r="B246" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D246" s="1"/>
+      <c r="E246" s="2">
+        <v>255</v>
+      </c>
+      <c r="F246" s="2">
+        <v>10</v>
+      </c>
+      <c r="G246" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A247" s="2">
+        <v>246</v>
+      </c>
+      <c r="B247" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D247" s="1"/>
+      <c r="E247" s="2">
+        <v>256</v>
+      </c>
+      <c r="F247" s="2">
+        <v>10</v>
+      </c>
+      <c r="G247" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A248" s="2">
+        <v>247</v>
+      </c>
+      <c r="B248" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D248" s="1"/>
+      <c r="E248" s="2">
+        <v>257</v>
+      </c>
+      <c r="F248" s="2">
+        <v>10</v>
+      </c>
+      <c r="G248" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A249" s="2">
+        <v>248</v>
+      </c>
+      <c r="B249" s="3">
+        <v>43237</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D249" s="1"/>
+      <c r="E249" s="2">
+        <v>258</v>
+      </c>
+      <c r="F249" s="2">
+        <v>10</v>
+      </c>
+      <c r="G249" s="2">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
datos para la revision ordinaria
</commit_message>
<xml_diff>
--- a/Datos/incidencia.xlsx
+++ b/Datos/incidencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33321899-ABF6-46B6-BD65-E69804AC4735}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A0FF2163-C38D-4F05-A66E-5C2602823E2F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="incidencia" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="12">
   <si>
     <t>idincidencia</t>
   </si>
@@ -391,7 +391,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -521,17 +521,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -577,7 +566,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -591,17 +580,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -959,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G250"/>
+  <dimension ref="A1:G249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="G250" sqref="G250"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2950,10 +2929,10 @@
       <c r="A95" s="4">
         <v>94</v>
       </c>
-      <c r="B95" s="5">
-        <v>43229</v>
-      </c>
-      <c r="C95" s="6" t="s">
+      <c r="B95" s="3">
+        <v>43236</v>
+      </c>
+      <c r="C95" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D95" s="1"/>
@@ -2961,7 +2940,7 @@
         <v>1</v>
       </c>
       <c r="F95" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G95" s="4">
         <v>4</v>
@@ -2972,7 +2951,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>11</v>
@@ -2981,8 +2960,8 @@
       <c r="E96" s="2">
         <v>2</v>
       </c>
-      <c r="F96" s="2">
-        <v>9</v>
+      <c r="F96" s="4">
+        <v>10</v>
       </c>
       <c r="G96" s="2">
         <v>1</v>
@@ -2993,7 +2972,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>11</v>
@@ -3002,8 +2981,8 @@
       <c r="E97" s="2">
         <v>3</v>
       </c>
-      <c r="F97" s="2">
-        <v>9</v>
+      <c r="F97" s="4">
+        <v>10</v>
       </c>
       <c r="G97" s="2">
         <v>1</v>
@@ -3014,7 +2993,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>11</v>
@@ -3023,8 +3002,8 @@
       <c r="E98" s="2">
         <v>4</v>
       </c>
-      <c r="F98" s="2">
-        <v>9</v>
+      <c r="F98" s="4">
+        <v>10</v>
       </c>
       <c r="G98" s="2">
         <v>1</v>
@@ -3035,7 +3014,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>11</v>
@@ -3044,8 +3023,8 @@
       <c r="E99" s="2">
         <v>5</v>
       </c>
-      <c r="F99" s="2">
-        <v>9</v>
+      <c r="F99" s="4">
+        <v>10</v>
       </c>
       <c r="G99" s="2">
         <v>1</v>
@@ -3056,7 +3035,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>11</v>
@@ -3065,8 +3044,8 @@
       <c r="E100" s="2">
         <v>6</v>
       </c>
-      <c r="F100" s="2">
-        <v>9</v>
+      <c r="F100" s="4">
+        <v>10</v>
       </c>
       <c r="G100" s="2">
         <v>1</v>
@@ -3077,7 +3056,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>11</v>
@@ -3086,8 +3065,8 @@
       <c r="E101" s="2">
         <v>7</v>
       </c>
-      <c r="F101" s="2">
-        <v>9</v>
+      <c r="F101" s="4">
+        <v>10</v>
       </c>
       <c r="G101" s="2">
         <v>1</v>
@@ -3098,7 +3077,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>11</v>
@@ -3107,8 +3086,8 @@
       <c r="E102" s="2">
         <v>8</v>
       </c>
-      <c r="F102" s="2">
-        <v>9</v>
+      <c r="F102" s="4">
+        <v>10</v>
       </c>
       <c r="G102" s="2">
         <v>1</v>
@@ -3119,7 +3098,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>11</v>
@@ -3128,8 +3107,8 @@
       <c r="E103" s="2">
         <v>9</v>
       </c>
-      <c r="F103" s="2">
-        <v>9</v>
+      <c r="F103" s="4">
+        <v>10</v>
       </c>
       <c r="G103" s="2">
         <v>1</v>
@@ -3140,7 +3119,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>7</v>
@@ -3149,8 +3128,8 @@
       <c r="E104" s="2">
         <v>10</v>
       </c>
-      <c r="F104" s="2">
-        <v>9</v>
+      <c r="F104" s="4">
+        <v>10</v>
       </c>
       <c r="G104" s="2">
         <v>3</v>
@@ -3161,7 +3140,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>7</v>
@@ -3170,8 +3149,8 @@
       <c r="E105" s="2">
         <v>11</v>
       </c>
-      <c r="F105" s="2">
-        <v>9</v>
+      <c r="F105" s="4">
+        <v>10</v>
       </c>
       <c r="G105" s="2">
         <v>3</v>
@@ -3182,7 +3161,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>7</v>
@@ -3191,8 +3170,8 @@
       <c r="E106" s="2">
         <v>12</v>
       </c>
-      <c r="F106" s="2">
-        <v>9</v>
+      <c r="F106" s="4">
+        <v>10</v>
       </c>
       <c r="G106" s="2">
         <v>4</v>
@@ -3203,7 +3182,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>7</v>
@@ -3212,8 +3191,8 @@
       <c r="E107" s="2">
         <v>13</v>
       </c>
-      <c r="F107" s="2">
-        <v>9</v>
+      <c r="F107" s="4">
+        <v>10</v>
       </c>
       <c r="G107" s="2">
         <v>4</v>
@@ -3224,7 +3203,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>7</v>
@@ -3233,8 +3212,8 @@
       <c r="E108" s="2">
         <v>14</v>
       </c>
-      <c r="F108" s="2">
-        <v>9</v>
+      <c r="F108" s="4">
+        <v>10</v>
       </c>
       <c r="G108" s="2">
         <v>5</v>
@@ -3245,7 +3224,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>7</v>
@@ -3254,8 +3233,8 @@
       <c r="E109" s="2">
         <v>15</v>
       </c>
-      <c r="F109" s="2">
-        <v>9</v>
+      <c r="F109" s="4">
+        <v>10</v>
       </c>
       <c r="G109" s="2">
         <v>5</v>
@@ -3266,7 +3245,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>7</v>
@@ -3275,8 +3254,8 @@
       <c r="E110" s="2">
         <v>243</v>
       </c>
-      <c r="F110" s="2">
-        <v>9</v>
+      <c r="F110" s="4">
+        <v>10</v>
       </c>
       <c r="G110" s="2">
         <v>1</v>
@@ -3287,7 +3266,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>7</v>
@@ -3296,8 +3275,8 @@
       <c r="E111" s="2">
         <v>244</v>
       </c>
-      <c r="F111" s="2">
-        <v>9</v>
+      <c r="F111" s="4">
+        <v>10</v>
       </c>
       <c r="G111" s="2">
         <v>1</v>
@@ -3308,7 +3287,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>7</v>
@@ -3317,8 +3296,8 @@
       <c r="E112" s="2">
         <v>245</v>
       </c>
-      <c r="F112" s="2">
-        <v>9</v>
+      <c r="F112" s="4">
+        <v>10</v>
       </c>
       <c r="G112" s="2">
         <v>1</v>
@@ -3329,7 +3308,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>7</v>
@@ -3338,8 +3317,8 @@
       <c r="E113" s="2">
         <v>246</v>
       </c>
-      <c r="F113" s="2">
-        <v>9</v>
+      <c r="F113" s="4">
+        <v>10</v>
       </c>
       <c r="G113" s="2">
         <v>1</v>
@@ -3350,7 +3329,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>7</v>
@@ -3359,8 +3338,8 @@
       <c r="E114" s="2">
         <v>247</v>
       </c>
-      <c r="F114" s="2">
-        <v>9</v>
+      <c r="F114" s="4">
+        <v>10</v>
       </c>
       <c r="G114" s="2">
         <v>1</v>
@@ -3371,7 +3350,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>7</v>
@@ -3380,8 +3359,8 @@
       <c r="E115" s="2">
         <v>248</v>
       </c>
-      <c r="F115" s="2">
-        <v>9</v>
+      <c r="F115" s="4">
+        <v>10</v>
       </c>
       <c r="G115" s="2">
         <v>1</v>
@@ -3392,7 +3371,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>7</v>
@@ -3401,8 +3380,8 @@
       <c r="E116" s="2">
         <v>249</v>
       </c>
-      <c r="F116" s="2">
-        <v>9</v>
+      <c r="F116" s="4">
+        <v>10</v>
       </c>
       <c r="G116" s="2">
         <v>1</v>
@@ -3413,7 +3392,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>7</v>
@@ -3422,8 +3401,8 @@
       <c r="E117" s="2">
         <v>250</v>
       </c>
-      <c r="F117" s="2">
-        <v>9</v>
+      <c r="F117" s="4">
+        <v>10</v>
       </c>
       <c r="G117" s="2">
         <v>1</v>
@@ -3434,7 +3413,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>7</v>
@@ -3443,8 +3422,8 @@
       <c r="E118" s="2">
         <v>251</v>
       </c>
-      <c r="F118" s="2">
-        <v>9</v>
+      <c r="F118" s="4">
+        <v>10</v>
       </c>
       <c r="G118" s="2">
         <v>1</v>
@@ -3455,7 +3434,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>7</v>
@@ -3464,8 +3443,8 @@
       <c r="E119" s="2">
         <v>252</v>
       </c>
-      <c r="F119" s="2">
-        <v>9</v>
+      <c r="F119" s="4">
+        <v>10</v>
       </c>
       <c r="G119" s="2">
         <v>1</v>
@@ -3476,7 +3455,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>7</v>
@@ -3485,8 +3464,8 @@
       <c r="E120" s="2">
         <v>253</v>
       </c>
-      <c r="F120" s="2">
-        <v>9</v>
+      <c r="F120" s="4">
+        <v>10</v>
       </c>
       <c r="G120" s="2">
         <v>1</v>
@@ -3497,7 +3476,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>7</v>
@@ -3506,8 +3485,8 @@
       <c r="E121" s="2">
         <v>254</v>
       </c>
-      <c r="F121" s="2">
-        <v>9</v>
+      <c r="F121" s="4">
+        <v>10</v>
       </c>
       <c r="G121" s="2">
         <v>1</v>
@@ -3518,7 +3497,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>8</v>
@@ -3527,8 +3506,8 @@
       <c r="E122" s="2">
         <v>255</v>
       </c>
-      <c r="F122" s="2">
-        <v>9</v>
+      <c r="F122" s="4">
+        <v>10</v>
       </c>
       <c r="G122" s="2">
         <v>0</v>
@@ -3539,7 +3518,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>8</v>
@@ -3548,8 +3527,8 @@
       <c r="E123" s="2">
         <v>256</v>
       </c>
-      <c r="F123" s="2">
-        <v>9</v>
+      <c r="F123" s="4">
+        <v>10</v>
       </c>
       <c r="G123" s="2">
         <v>0</v>
@@ -3560,7 +3539,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>8</v>
@@ -3569,8 +3548,8 @@
       <c r="E124" s="2">
         <v>257</v>
       </c>
-      <c r="F124" s="2">
-        <v>9</v>
+      <c r="F124" s="4">
+        <v>10</v>
       </c>
       <c r="G124" s="2">
         <v>0</v>
@@ -3581,7 +3560,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="3">
-        <v>43229</v>
+        <v>43236</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>8</v>
@@ -3590,8 +3569,8 @@
       <c r="E125" s="2">
         <v>258</v>
       </c>
-      <c r="F125" s="2">
-        <v>9</v>
+      <c r="F125" s="4">
+        <v>10</v>
       </c>
       <c r="G125" s="2">
         <v>0</v>
@@ -3602,17 +3581,17 @@
         <v>125</v>
       </c>
       <c r="B126" s="3">
-        <v>43230</v>
-      </c>
-      <c r="C126" s="6" t="s">
+        <v>43237</v>
+      </c>
+      <c r="C126" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D126" s="1"/>
       <c r="E126" s="2">
         <v>1</v>
       </c>
-      <c r="F126" s="2">
-        <v>9</v>
+      <c r="F126" s="4">
+        <v>10</v>
       </c>
       <c r="G126" s="4">
         <v>4</v>
@@ -3623,7 +3602,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>11</v>
@@ -3632,8 +3611,8 @@
       <c r="E127" s="2">
         <v>2</v>
       </c>
-      <c r="F127" s="2">
-        <v>9</v>
+      <c r="F127" s="4">
+        <v>10</v>
       </c>
       <c r="G127" s="2">
         <v>1</v>
@@ -3644,7 +3623,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>11</v>
@@ -3653,8 +3632,8 @@
       <c r="E128" s="2">
         <v>3</v>
       </c>
-      <c r="F128" s="2">
-        <v>9</v>
+      <c r="F128" s="4">
+        <v>10</v>
       </c>
       <c r="G128" s="2">
         <v>1</v>
@@ -3665,7 +3644,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>11</v>
@@ -3674,8 +3653,8 @@
       <c r="E129" s="2">
         <v>4</v>
       </c>
-      <c r="F129" s="2">
-        <v>9</v>
+      <c r="F129" s="4">
+        <v>10</v>
       </c>
       <c r="G129" s="2">
         <v>1</v>
@@ -3686,7 +3665,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>11</v>
@@ -3695,8 +3674,8 @@
       <c r="E130" s="2">
         <v>5</v>
       </c>
-      <c r="F130" s="2">
-        <v>9</v>
+      <c r="F130" s="4">
+        <v>10</v>
       </c>
       <c r="G130" s="2">
         <v>1</v>
@@ -3707,7 +3686,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>11</v>
@@ -3716,8 +3695,8 @@
       <c r="E131" s="2">
         <v>6</v>
       </c>
-      <c r="F131" s="2">
-        <v>9</v>
+      <c r="F131" s="4">
+        <v>10</v>
       </c>
       <c r="G131" s="2">
         <v>1</v>
@@ -3728,7 +3707,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>11</v>
@@ -3737,8 +3716,8 @@
       <c r="E132" s="2">
         <v>7</v>
       </c>
-      <c r="F132" s="2">
-        <v>9</v>
+      <c r="F132" s="4">
+        <v>10</v>
       </c>
       <c r="G132" s="2">
         <v>1</v>
@@ -3749,7 +3728,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>11</v>
@@ -3758,8 +3737,8 @@
       <c r="E133" s="2">
         <v>8</v>
       </c>
-      <c r="F133" s="2">
-        <v>9</v>
+      <c r="F133" s="4">
+        <v>10</v>
       </c>
       <c r="G133" s="2">
         <v>1</v>
@@ -3770,7 +3749,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>11</v>
@@ -3779,8 +3758,8 @@
       <c r="E134" s="2">
         <v>9</v>
       </c>
-      <c r="F134" s="2">
-        <v>9</v>
+      <c r="F134" s="4">
+        <v>10</v>
       </c>
       <c r="G134" s="2">
         <v>1</v>
@@ -3791,7 +3770,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>7</v>
@@ -3800,8 +3779,8 @@
       <c r="E135" s="2">
         <v>10</v>
       </c>
-      <c r="F135" s="2">
-        <v>9</v>
+      <c r="F135" s="4">
+        <v>10</v>
       </c>
       <c r="G135" s="2">
         <v>3</v>
@@ -3812,7 +3791,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>7</v>
@@ -3821,8 +3800,8 @@
       <c r="E136" s="2">
         <v>11</v>
       </c>
-      <c r="F136" s="2">
-        <v>9</v>
+      <c r="F136" s="4">
+        <v>10</v>
       </c>
       <c r="G136" s="2">
         <v>3</v>
@@ -3833,7 +3812,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>7</v>
@@ -3842,8 +3821,8 @@
       <c r="E137" s="2">
         <v>12</v>
       </c>
-      <c r="F137" s="2">
-        <v>9</v>
+      <c r="F137" s="4">
+        <v>10</v>
       </c>
       <c r="G137" s="2">
         <v>4</v>
@@ -3854,7 +3833,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>7</v>
@@ -3863,8 +3842,8 @@
       <c r="E138" s="2">
         <v>13</v>
       </c>
-      <c r="F138" s="2">
-        <v>9</v>
+      <c r="F138" s="4">
+        <v>10</v>
       </c>
       <c r="G138" s="2">
         <v>4</v>
@@ -3875,7 +3854,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>7</v>
@@ -3884,8 +3863,8 @@
       <c r="E139" s="2">
         <v>14</v>
       </c>
-      <c r="F139" s="2">
-        <v>9</v>
+      <c r="F139" s="4">
+        <v>10</v>
       </c>
       <c r="G139" s="2">
         <v>5</v>
@@ -3896,7 +3875,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>7</v>
@@ -3905,8 +3884,8 @@
       <c r="E140" s="2">
         <v>15</v>
       </c>
-      <c r="F140" s="2">
-        <v>9</v>
+      <c r="F140" s="4">
+        <v>10</v>
       </c>
       <c r="G140" s="2">
         <v>5</v>
@@ -3917,7 +3896,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>7</v>
@@ -3926,8 +3905,8 @@
       <c r="E141" s="2">
         <v>243</v>
       </c>
-      <c r="F141" s="2">
-        <v>9</v>
+      <c r="F141" s="4">
+        <v>10</v>
       </c>
       <c r="G141" s="2">
         <v>1</v>
@@ -3938,7 +3917,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>7</v>
@@ -3947,8 +3926,8 @@
       <c r="E142" s="2">
         <v>244</v>
       </c>
-      <c r="F142" s="2">
-        <v>9</v>
+      <c r="F142" s="4">
+        <v>10</v>
       </c>
       <c r="G142" s="2">
         <v>1</v>
@@ -3959,7 +3938,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>7</v>
@@ -3968,8 +3947,8 @@
       <c r="E143" s="2">
         <v>245</v>
       </c>
-      <c r="F143" s="2">
-        <v>9</v>
+      <c r="F143" s="4">
+        <v>10</v>
       </c>
       <c r="G143" s="2">
         <v>1</v>
@@ -3980,7 +3959,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>7</v>
@@ -3989,8 +3968,8 @@
       <c r="E144" s="2">
         <v>246</v>
       </c>
-      <c r="F144" s="2">
-        <v>9</v>
+      <c r="F144" s="4">
+        <v>10</v>
       </c>
       <c r="G144" s="2">
         <v>1</v>
@@ -4001,7 +3980,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>7</v>
@@ -4010,8 +3989,8 @@
       <c r="E145" s="2">
         <v>247</v>
       </c>
-      <c r="F145" s="2">
-        <v>9</v>
+      <c r="F145" s="4">
+        <v>10</v>
       </c>
       <c r="G145" s="2">
         <v>1</v>
@@ -4022,7 +4001,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>7</v>
@@ -4031,8 +4010,8 @@
       <c r="E146" s="2">
         <v>248</v>
       </c>
-      <c r="F146" s="2">
-        <v>9</v>
+      <c r="F146" s="4">
+        <v>10</v>
       </c>
       <c r="G146" s="2">
         <v>1</v>
@@ -4043,7 +4022,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>7</v>
@@ -4052,8 +4031,8 @@
       <c r="E147" s="2">
         <v>249</v>
       </c>
-      <c r="F147" s="2">
-        <v>9</v>
+      <c r="F147" s="4">
+        <v>10</v>
       </c>
       <c r="G147" s="2">
         <v>1</v>
@@ -4064,7 +4043,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>7</v>
@@ -4073,8 +4052,8 @@
       <c r="E148" s="2">
         <v>250</v>
       </c>
-      <c r="F148" s="2">
-        <v>9</v>
+      <c r="F148" s="4">
+        <v>10</v>
       </c>
       <c r="G148" s="2">
         <v>1</v>
@@ -4085,7 +4064,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>7</v>
@@ -4094,8 +4073,8 @@
       <c r="E149" s="2">
         <v>251</v>
       </c>
-      <c r="F149" s="2">
-        <v>9</v>
+      <c r="F149" s="4">
+        <v>10</v>
       </c>
       <c r="G149" s="2">
         <v>1</v>
@@ -4106,7 +4085,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>7</v>
@@ -4115,8 +4094,8 @@
       <c r="E150" s="2">
         <v>252</v>
       </c>
-      <c r="F150" s="2">
-        <v>9</v>
+      <c r="F150" s="4">
+        <v>10</v>
       </c>
       <c r="G150" s="2">
         <v>1</v>
@@ -4127,7 +4106,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>7</v>
@@ -4136,8 +4115,8 @@
       <c r="E151" s="2">
         <v>253</v>
       </c>
-      <c r="F151" s="2">
-        <v>9</v>
+      <c r="F151" s="4">
+        <v>10</v>
       </c>
       <c r="G151" s="2">
         <v>1</v>
@@ -4148,7 +4127,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>7</v>
@@ -4157,8 +4136,8 @@
       <c r="E152" s="2">
         <v>254</v>
       </c>
-      <c r="F152" s="2">
-        <v>9</v>
+      <c r="F152" s="4">
+        <v>10</v>
       </c>
       <c r="G152" s="2">
         <v>1</v>
@@ -4169,7 +4148,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>9</v>
@@ -4178,8 +4157,8 @@
       <c r="E153" s="2">
         <v>255</v>
       </c>
-      <c r="F153" s="2">
-        <v>9</v>
+      <c r="F153" s="4">
+        <v>10</v>
       </c>
       <c r="G153" s="2">
         <v>1</v>
@@ -4190,7 +4169,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>9</v>
@@ -4199,8 +4178,8 @@
       <c r="E154" s="2">
         <v>256</v>
       </c>
-      <c r="F154" s="2">
-        <v>9</v>
+      <c r="F154" s="4">
+        <v>10</v>
       </c>
       <c r="G154" s="2">
         <v>1</v>
@@ -4211,7 +4190,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>9</v>
@@ -4220,8 +4199,8 @@
       <c r="E155" s="2">
         <v>257</v>
       </c>
-      <c r="F155" s="2">
-        <v>9</v>
+      <c r="F155" s="4">
+        <v>10</v>
       </c>
       <c r="G155" s="2">
         <v>1</v>
@@ -4232,7 +4211,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="3">
-        <v>43230</v>
+        <v>43237</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>9</v>
@@ -4241,8 +4220,8 @@
       <c r="E156" s="2">
         <v>258</v>
       </c>
-      <c r="F156" s="2">
-        <v>9</v>
+      <c r="F156" s="4">
+        <v>10</v>
       </c>
       <c r="G156" s="2">
         <v>1</v>
@@ -4253,17 +4232,17 @@
         <v>156</v>
       </c>
       <c r="B157" s="3">
-        <v>43234</v>
-      </c>
-      <c r="C157" s="6" t="s">
+        <v>43238</v>
+      </c>
+      <c r="C157" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D157" s="1"/>
       <c r="E157" s="2">
         <v>1</v>
       </c>
-      <c r="F157" s="2">
-        <v>9</v>
+      <c r="F157" s="4">
+        <v>10</v>
       </c>
       <c r="G157" s="4">
         <v>4</v>
@@ -4274,7 +4253,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>11</v>
@@ -4283,8 +4262,8 @@
       <c r="E158" s="2">
         <v>2</v>
       </c>
-      <c r="F158" s="2">
-        <v>9</v>
+      <c r="F158" s="4">
+        <v>10</v>
       </c>
       <c r="G158" s="2">
         <v>1</v>
@@ -4295,7 +4274,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>11</v>
@@ -4304,8 +4283,8 @@
       <c r="E159" s="2">
         <v>3</v>
       </c>
-      <c r="F159" s="2">
-        <v>9</v>
+      <c r="F159" s="4">
+        <v>10</v>
       </c>
       <c r="G159" s="2">
         <v>1</v>
@@ -4316,7 +4295,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>11</v>
@@ -4325,8 +4304,8 @@
       <c r="E160" s="2">
         <v>4</v>
       </c>
-      <c r="F160" s="2">
-        <v>9</v>
+      <c r="F160" s="4">
+        <v>10</v>
       </c>
       <c r="G160" s="2">
         <v>1</v>
@@ -4337,7 +4316,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>11</v>
@@ -4346,8 +4325,8 @@
       <c r="E161" s="2">
         <v>5</v>
       </c>
-      <c r="F161" s="2">
-        <v>9</v>
+      <c r="F161" s="4">
+        <v>10</v>
       </c>
       <c r="G161" s="2">
         <v>1</v>
@@ -4358,7 +4337,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>11</v>
@@ -4367,8 +4346,8 @@
       <c r="E162" s="2">
         <v>6</v>
       </c>
-      <c r="F162" s="2">
-        <v>9</v>
+      <c r="F162" s="4">
+        <v>10</v>
       </c>
       <c r="G162" s="2">
         <v>1</v>
@@ -4379,7 +4358,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>11</v>
@@ -4388,8 +4367,8 @@
       <c r="E163" s="2">
         <v>7</v>
       </c>
-      <c r="F163" s="2">
-        <v>9</v>
+      <c r="F163" s="4">
+        <v>10</v>
       </c>
       <c r="G163" s="2">
         <v>1</v>
@@ -4400,7 +4379,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>11</v>
@@ -4409,8 +4388,8 @@
       <c r="E164" s="2">
         <v>8</v>
       </c>
-      <c r="F164" s="2">
-        <v>9</v>
+      <c r="F164" s="4">
+        <v>10</v>
       </c>
       <c r="G164" s="2">
         <v>1</v>
@@ -4421,7 +4400,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>11</v>
@@ -4430,8 +4409,8 @@
       <c r="E165" s="2">
         <v>9</v>
       </c>
-      <c r="F165" s="2">
-        <v>9</v>
+      <c r="F165" s="4">
+        <v>10</v>
       </c>
       <c r="G165" s="2">
         <v>1</v>
@@ -4442,7 +4421,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>7</v>
@@ -4451,8 +4430,8 @@
       <c r="E166" s="2">
         <v>10</v>
       </c>
-      <c r="F166" s="2">
-        <v>9</v>
+      <c r="F166" s="4">
+        <v>10</v>
       </c>
       <c r="G166" s="2">
         <v>3</v>
@@ -4463,7 +4442,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>7</v>
@@ -4472,8 +4451,8 @@
       <c r="E167" s="2">
         <v>11</v>
       </c>
-      <c r="F167" s="2">
-        <v>9</v>
+      <c r="F167" s="4">
+        <v>10</v>
       </c>
       <c r="G167" s="2">
         <v>3</v>
@@ -4484,7 +4463,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>7</v>
@@ -4493,8 +4472,8 @@
       <c r="E168" s="2">
         <v>12</v>
       </c>
-      <c r="F168" s="2">
-        <v>9</v>
+      <c r="F168" s="4">
+        <v>10</v>
       </c>
       <c r="G168" s="2">
         <v>4</v>
@@ -4505,7 +4484,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>7</v>
@@ -4514,8 +4493,8 @@
       <c r="E169" s="2">
         <v>13</v>
       </c>
-      <c r="F169" s="2">
-        <v>9</v>
+      <c r="F169" s="4">
+        <v>10</v>
       </c>
       <c r="G169" s="2">
         <v>4</v>
@@ -4526,7 +4505,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>7</v>
@@ -4535,8 +4514,8 @@
       <c r="E170" s="2">
         <v>14</v>
       </c>
-      <c r="F170" s="2">
-        <v>9</v>
+      <c r="F170" s="4">
+        <v>10</v>
       </c>
       <c r="G170" s="2">
         <v>5</v>
@@ -4547,7 +4526,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>7</v>
@@ -4556,8 +4535,8 @@
       <c r="E171" s="2">
         <v>15</v>
       </c>
-      <c r="F171" s="2">
-        <v>9</v>
+      <c r="F171" s="4">
+        <v>10</v>
       </c>
       <c r="G171" s="2">
         <v>5</v>
@@ -4568,7 +4547,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>7</v>
@@ -4577,8 +4556,8 @@
       <c r="E172" s="2">
         <v>243</v>
       </c>
-      <c r="F172" s="2">
-        <v>9</v>
+      <c r="F172" s="4">
+        <v>10</v>
       </c>
       <c r="G172" s="2">
         <v>1</v>
@@ -4589,7 +4568,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>7</v>
@@ -4598,8 +4577,8 @@
       <c r="E173" s="2">
         <v>244</v>
       </c>
-      <c r="F173" s="2">
-        <v>9</v>
+      <c r="F173" s="4">
+        <v>10</v>
       </c>
       <c r="G173" s="2">
         <v>1</v>
@@ -4610,7 +4589,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>7</v>
@@ -4619,8 +4598,8 @@
       <c r="E174" s="2">
         <v>245</v>
       </c>
-      <c r="F174" s="2">
-        <v>9</v>
+      <c r="F174" s="4">
+        <v>10</v>
       </c>
       <c r="G174" s="2">
         <v>1</v>
@@ -4631,7 +4610,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>7</v>
@@ -4640,8 +4619,8 @@
       <c r="E175" s="2">
         <v>246</v>
       </c>
-      <c r="F175" s="2">
-        <v>9</v>
+      <c r="F175" s="4">
+        <v>10</v>
       </c>
       <c r="G175" s="2">
         <v>1</v>
@@ -4652,7 +4631,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>7</v>
@@ -4661,8 +4640,8 @@
       <c r="E176" s="2">
         <v>247</v>
       </c>
-      <c r="F176" s="2">
-        <v>9</v>
+      <c r="F176" s="4">
+        <v>10</v>
       </c>
       <c r="G176" s="2">
         <v>1</v>
@@ -4673,7 +4652,7 @@
         <v>176</v>
       </c>
       <c r="B177" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>7</v>
@@ -4682,8 +4661,8 @@
       <c r="E177" s="2">
         <v>248</v>
       </c>
-      <c r="F177" s="2">
-        <v>9</v>
+      <c r="F177" s="4">
+        <v>10</v>
       </c>
       <c r="G177" s="2">
         <v>1</v>
@@ -4694,7 +4673,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>7</v>
@@ -4703,8 +4682,8 @@
       <c r="E178" s="2">
         <v>249</v>
       </c>
-      <c r="F178" s="2">
-        <v>9</v>
+      <c r="F178" s="4">
+        <v>10</v>
       </c>
       <c r="G178" s="2">
         <v>1</v>
@@ -4715,7 +4694,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>7</v>
@@ -4724,8 +4703,8 @@
       <c r="E179" s="2">
         <v>250</v>
       </c>
-      <c r="F179" s="2">
-        <v>9</v>
+      <c r="F179" s="4">
+        <v>10</v>
       </c>
       <c r="G179" s="2">
         <v>1</v>
@@ -4736,7 +4715,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>7</v>
@@ -4745,8 +4724,8 @@
       <c r="E180" s="2">
         <v>251</v>
       </c>
-      <c r="F180" s="2">
-        <v>9</v>
+      <c r="F180" s="4">
+        <v>10</v>
       </c>
       <c r="G180" s="2">
         <v>1</v>
@@ -4757,7 +4736,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>7</v>
@@ -4766,8 +4745,8 @@
       <c r="E181" s="2">
         <v>252</v>
       </c>
-      <c r="F181" s="2">
-        <v>9</v>
+      <c r="F181" s="4">
+        <v>10</v>
       </c>
       <c r="G181" s="2">
         <v>1</v>
@@ -4778,7 +4757,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>7</v>
@@ -4787,8 +4766,8 @@
       <c r="E182" s="2">
         <v>253</v>
       </c>
-      <c r="F182" s="2">
-        <v>9</v>
+      <c r="F182" s="4">
+        <v>10</v>
       </c>
       <c r="G182" s="2">
         <v>1</v>
@@ -4799,7 +4778,7 @@
         <v>182</v>
       </c>
       <c r="B183" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>7</v>
@@ -4808,8 +4787,8 @@
       <c r="E183" s="2">
         <v>254</v>
       </c>
-      <c r="F183" s="2">
-        <v>9</v>
+      <c r="F183" s="4">
+        <v>10</v>
       </c>
       <c r="G183" s="2">
         <v>1</v>
@@ -4820,7 +4799,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>8</v>
@@ -4829,8 +4808,8 @@
       <c r="E184" s="2">
         <v>255</v>
       </c>
-      <c r="F184" s="2">
-        <v>9</v>
+      <c r="F184" s="4">
+        <v>10</v>
       </c>
       <c r="G184" s="2">
         <v>0</v>
@@ -4841,7 +4820,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>8</v>
@@ -4850,8 +4829,8 @@
       <c r="E185" s="2">
         <v>256</v>
       </c>
-      <c r="F185" s="2">
-        <v>9</v>
+      <c r="F185" s="4">
+        <v>10</v>
       </c>
       <c r="G185" s="2">
         <v>0</v>
@@ -4862,7 +4841,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>8</v>
@@ -4871,8 +4850,8 @@
       <c r="E186" s="2">
         <v>257</v>
       </c>
-      <c r="F186" s="2">
-        <v>9</v>
+      <c r="F186" s="4">
+        <v>10</v>
       </c>
       <c r="G186" s="2">
         <v>0</v>
@@ -4883,7 +4862,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="3">
-        <v>43234</v>
+        <v>43238</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>8</v>
@@ -4892,8 +4871,8 @@
       <c r="E187" s="2">
         <v>258</v>
       </c>
-      <c r="F187" s="2">
-        <v>9</v>
+      <c r="F187" s="4">
+        <v>10</v>
       </c>
       <c r="G187" s="2">
         <v>0</v>
@@ -4904,9 +4883,9 @@
         <v>187</v>
       </c>
       <c r="B188" s="3">
-        <v>43236</v>
-      </c>
-      <c r="C188" s="6" t="s">
+        <v>43255</v>
+      </c>
+      <c r="C188" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D188" s="1"/>
@@ -4914,7 +4893,7 @@
         <v>1</v>
       </c>
       <c r="F188" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G188" s="4">
         <v>4</v>
@@ -4925,7 +4904,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>11</v>
@@ -4935,7 +4914,7 @@
         <v>2</v>
       </c>
       <c r="F189" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G189" s="2">
         <v>1</v>
@@ -4946,7 +4925,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>11</v>
@@ -4956,7 +4935,7 @@
         <v>3</v>
       </c>
       <c r="F190" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G190" s="2">
         <v>1</v>
@@ -4967,7 +4946,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>11</v>
@@ -4977,7 +4956,7 @@
         <v>4</v>
       </c>
       <c r="F191" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G191" s="2">
         <v>1</v>
@@ -4988,7 +4967,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>11</v>
@@ -4998,7 +4977,7 @@
         <v>5</v>
       </c>
       <c r="F192" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G192" s="2">
         <v>1</v>
@@ -5009,7 +4988,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>11</v>
@@ -5019,7 +4998,7 @@
         <v>6</v>
       </c>
       <c r="F193" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G193" s="2">
         <v>1</v>
@@ -5030,7 +5009,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>11</v>
@@ -5040,7 +5019,7 @@
         <v>7</v>
       </c>
       <c r="F194" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G194" s="2">
         <v>1</v>
@@ -5051,7 +5030,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>11</v>
@@ -5061,7 +5040,7 @@
         <v>8</v>
       </c>
       <c r="F195" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G195" s="2">
         <v>1</v>
@@ -5072,7 +5051,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>11</v>
@@ -5082,7 +5061,7 @@
         <v>9</v>
       </c>
       <c r="F196" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G196" s="2">
         <v>1</v>
@@ -5093,7 +5072,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>7</v>
@@ -5103,7 +5082,7 @@
         <v>10</v>
       </c>
       <c r="F197" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G197" s="2">
         <v>3</v>
@@ -5114,7 +5093,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>7</v>
@@ -5124,7 +5103,7 @@
         <v>11</v>
       </c>
       <c r="F198" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G198" s="2">
         <v>3</v>
@@ -5135,7 +5114,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>7</v>
@@ -5145,7 +5124,7 @@
         <v>12</v>
       </c>
       <c r="F199" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G199" s="2">
         <v>4</v>
@@ -5156,7 +5135,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>7</v>
@@ -5166,7 +5145,7 @@
         <v>13</v>
       </c>
       <c r="F200" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G200" s="2">
         <v>4</v>
@@ -5177,7 +5156,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>7</v>
@@ -5187,7 +5166,7 @@
         <v>14</v>
       </c>
       <c r="F201" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G201" s="2">
         <v>5</v>
@@ -5198,7 +5177,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>7</v>
@@ -5208,7 +5187,7 @@
         <v>15</v>
       </c>
       <c r="F202" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G202" s="2">
         <v>5</v>
@@ -5219,7 +5198,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>7</v>
@@ -5229,7 +5208,7 @@
         <v>243</v>
       </c>
       <c r="F203" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G203" s="2">
         <v>1</v>
@@ -5240,7 +5219,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>7</v>
@@ -5250,7 +5229,7 @@
         <v>244</v>
       </c>
       <c r="F204" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G204" s="2">
         <v>1</v>
@@ -5261,7 +5240,7 @@
         <v>204</v>
       </c>
       <c r="B205" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>7</v>
@@ -5271,7 +5250,7 @@
         <v>245</v>
       </c>
       <c r="F205" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G205" s="2">
         <v>1</v>
@@ -5282,7 +5261,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>7</v>
@@ -5292,7 +5271,7 @@
         <v>246</v>
       </c>
       <c r="F206" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G206" s="2">
         <v>1</v>
@@ -5303,7 +5282,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>7</v>
@@ -5313,7 +5292,7 @@
         <v>247</v>
       </c>
       <c r="F207" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G207" s="2">
         <v>1</v>
@@ -5324,7 +5303,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>7</v>
@@ -5334,7 +5313,7 @@
         <v>248</v>
       </c>
       <c r="F208" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G208" s="2">
         <v>1</v>
@@ -5345,7 +5324,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>7</v>
@@ -5355,7 +5334,7 @@
         <v>249</v>
       </c>
       <c r="F209" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G209" s="2">
         <v>1</v>
@@ -5366,7 +5345,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>7</v>
@@ -5376,7 +5355,7 @@
         <v>250</v>
       </c>
       <c r="F210" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G210" s="2">
         <v>1</v>
@@ -5387,7 +5366,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>7</v>
@@ -5397,7 +5376,7 @@
         <v>251</v>
       </c>
       <c r="F211" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G211" s="2">
         <v>1</v>
@@ -5408,7 +5387,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>7</v>
@@ -5418,7 +5397,7 @@
         <v>252</v>
       </c>
       <c r="F212" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G212" s="2">
         <v>1</v>
@@ -5429,7 +5408,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>7</v>
@@ -5439,7 +5418,7 @@
         <v>253</v>
       </c>
       <c r="F213" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G213" s="2">
         <v>1</v>
@@ -5450,7 +5429,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>7</v>
@@ -5460,7 +5439,7 @@
         <v>254</v>
       </c>
       <c r="F214" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G214" s="2">
         <v>1</v>
@@ -5471,7 +5450,7 @@
         <v>214</v>
       </c>
       <c r="B215" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>8</v>
@@ -5481,7 +5460,7 @@
         <v>255</v>
       </c>
       <c r="F215" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G215" s="2">
         <v>0</v>
@@ -5492,7 +5471,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>8</v>
@@ -5502,7 +5481,7 @@
         <v>256</v>
       </c>
       <c r="F216" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G216" s="2">
         <v>0</v>
@@ -5513,7 +5492,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>8</v>
@@ -5523,7 +5502,7 @@
         <v>257</v>
       </c>
       <c r="F217" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G217" s="2">
         <v>0</v>
@@ -5534,7 +5513,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="3">
-        <v>43236</v>
+        <v>43255</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>8</v>
@@ -5544,7 +5523,7 @@
         <v>258</v>
       </c>
       <c r="F218" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G218" s="2">
         <v>0</v>
@@ -5555,9 +5534,9 @@
         <v>218</v>
       </c>
       <c r="B219" s="3">
-        <v>43237</v>
-      </c>
-      <c r="C219" s="6" t="s">
+        <v>43256</v>
+      </c>
+      <c r="C219" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D219" s="1"/>
@@ -5565,7 +5544,7 @@
         <v>1</v>
       </c>
       <c r="F219" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G219" s="4">
         <v>4</v>
@@ -5576,7 +5555,7 @@
         <v>219</v>
       </c>
       <c r="B220" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>11</v>
@@ -5586,7 +5565,7 @@
         <v>2</v>
       </c>
       <c r="F220" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G220" s="2">
         <v>1</v>
@@ -5597,7 +5576,7 @@
         <v>220</v>
       </c>
       <c r="B221" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>11</v>
@@ -5607,7 +5586,7 @@
         <v>3</v>
       </c>
       <c r="F221" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G221" s="2">
         <v>1</v>
@@ -5618,7 +5597,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>11</v>
@@ -5628,7 +5607,7 @@
         <v>4</v>
       </c>
       <c r="F222" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G222" s="2">
         <v>1</v>
@@ -5639,7 +5618,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>11</v>
@@ -5649,7 +5628,7 @@
         <v>5</v>
       </c>
       <c r="F223" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G223" s="2">
         <v>1</v>
@@ -5660,7 +5639,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>11</v>
@@ -5670,7 +5649,7 @@
         <v>6</v>
       </c>
       <c r="F224" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G224" s="2">
         <v>1</v>
@@ -5681,7 +5660,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>11</v>
@@ -5691,7 +5670,7 @@
         <v>7</v>
       </c>
       <c r="F225" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G225" s="2">
         <v>1</v>
@@ -5702,7 +5681,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>11</v>
@@ -5712,7 +5691,7 @@
         <v>8</v>
       </c>
       <c r="F226" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G226" s="2">
         <v>1</v>
@@ -5723,7 +5702,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>11</v>
@@ -5733,7 +5712,7 @@
         <v>9</v>
       </c>
       <c r="F227" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G227" s="2">
         <v>1</v>
@@ -5744,7 +5723,7 @@
         <v>227</v>
       </c>
       <c r="B228" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>7</v>
@@ -5754,7 +5733,7 @@
         <v>10</v>
       </c>
       <c r="F228" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G228" s="2">
         <v>3</v>
@@ -5765,7 +5744,7 @@
         <v>228</v>
       </c>
       <c r="B229" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>7</v>
@@ -5775,7 +5754,7 @@
         <v>11</v>
       </c>
       <c r="F229" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G229" s="2">
         <v>3</v>
@@ -5786,7 +5765,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>7</v>
@@ -5796,7 +5775,7 @@
         <v>12</v>
       </c>
       <c r="F230" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G230" s="2">
         <v>4</v>
@@ -5807,7 +5786,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>7</v>
@@ -5817,7 +5796,7 @@
         <v>13</v>
       </c>
       <c r="F231" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G231" s="2">
         <v>4</v>
@@ -5828,7 +5807,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>7</v>
@@ -5838,7 +5817,7 @@
         <v>14</v>
       </c>
       <c r="F232" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G232" s="2">
         <v>5</v>
@@ -5849,7 +5828,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>7</v>
@@ -5859,7 +5838,7 @@
         <v>15</v>
       </c>
       <c r="F233" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G233" s="2">
         <v>5</v>
@@ -5870,7 +5849,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>7</v>
@@ -5880,7 +5859,7 @@
         <v>243</v>
       </c>
       <c r="F234" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G234" s="2">
         <v>1</v>
@@ -5891,7 +5870,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>7</v>
@@ -5901,7 +5880,7 @@
         <v>244</v>
       </c>
       <c r="F235" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G235" s="2">
         <v>1</v>
@@ -5912,7 +5891,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>7</v>
@@ -5922,7 +5901,7 @@
         <v>245</v>
       </c>
       <c r="F236" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G236" s="2">
         <v>1</v>
@@ -5933,7 +5912,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>7</v>
@@ -5943,7 +5922,7 @@
         <v>246</v>
       </c>
       <c r="F237" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G237" s="2">
         <v>1</v>
@@ -5954,7 +5933,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>7</v>
@@ -5964,7 +5943,7 @@
         <v>247</v>
       </c>
       <c r="F238" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G238" s="2">
         <v>1</v>
@@ -5975,7 +5954,7 @@
         <v>238</v>
       </c>
       <c r="B239" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>7</v>
@@ -5985,7 +5964,7 @@
         <v>248</v>
       </c>
       <c r="F239" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G239" s="2">
         <v>1</v>
@@ -5996,7 +5975,7 @@
         <v>239</v>
       </c>
       <c r="B240" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>7</v>
@@ -6006,7 +5985,7 @@
         <v>249</v>
       </c>
       <c r="F240" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G240" s="2">
         <v>1</v>
@@ -6017,7 +5996,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>7</v>
@@ -6027,7 +6006,7 @@
         <v>250</v>
       </c>
       <c r="F241" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G241" s="2">
         <v>1</v>
@@ -6038,7 +6017,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>7</v>
@@ -6048,7 +6027,7 @@
         <v>251</v>
       </c>
       <c r="F242" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G242" s="2">
         <v>1</v>
@@ -6059,7 +6038,7 @@
         <v>242</v>
       </c>
       <c r="B243" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>7</v>
@@ -6069,7 +6048,7 @@
         <v>252</v>
       </c>
       <c r="F243" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G243" s="2">
         <v>1</v>
@@ -6080,7 +6059,7 @@
         <v>243</v>
       </c>
       <c r="B244" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>7</v>
@@ -6090,7 +6069,7 @@
         <v>253</v>
       </c>
       <c r="F244" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G244" s="2">
         <v>1</v>
@@ -6101,7 +6080,7 @@
         <v>244</v>
       </c>
       <c r="B245" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>7</v>
@@ -6111,7 +6090,7 @@
         <v>254</v>
       </c>
       <c r="F245" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G245" s="2">
         <v>1</v>
@@ -6122,7 +6101,7 @@
         <v>245</v>
       </c>
       <c r="B246" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>9</v>
@@ -6132,7 +6111,7 @@
         <v>255</v>
       </c>
       <c r="F246" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G246" s="2">
         <v>6</v>
@@ -6143,7 +6122,7 @@
         <v>246</v>
       </c>
       <c r="B247" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>9</v>
@@ -6153,7 +6132,7 @@
         <v>256</v>
       </c>
       <c r="F247" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G247" s="2">
         <v>7</v>
@@ -6164,7 +6143,7 @@
         <v>247</v>
       </c>
       <c r="B248" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>9</v>
@@ -6174,7 +6153,7 @@
         <v>257</v>
       </c>
       <c r="F248" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G248" s="2">
         <v>7</v>
@@ -6185,7 +6164,7 @@
         <v>248</v>
       </c>
       <c r="B249" s="3">
-        <v>43237</v>
+        <v>43256</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>9</v>
@@ -6195,30 +6174,10 @@
         <v>258</v>
       </c>
       <c r="F249" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G249" s="2">
         <v>8</v>
-      </c>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A250" s="7">
-        <v>249</v>
-      </c>
-      <c r="B250" s="8">
-        <v>43238</v>
-      </c>
-      <c r="C250" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E250" s="7">
-        <v>16</v>
-      </c>
-      <c r="F250" s="7">
-        <v>10</v>
-      </c>
-      <c r="G250" s="7">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>